<commit_message>
[1D] Added number of pixels of color chosen.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hsdyn-my.sharepoint.com/personal/bmonteiro_hsdyn_com/Documents/Documents/IMAVD_GRUPO_IMAGEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F079DAE8-0ED3-4839-90F9-17A1B5E00BBC}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2EC6CBF-AE0C-47D0-ACF5-2A002B384297}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -277,6 +277,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,7 +549,7 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +566,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>8.3333333333333339</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -678,15 +682,14 @@
         <v>12</v>
       </c>
       <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
+        <v>100</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[1A] Implemented choosing color with mouse
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hsdyn-my.sharepoint.com/personal/bmonteiro_hsdyn_com/Documents/Documents/IMAVD_GRUPO_IMAGEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2EC6CBF-AE0C-47D0-ACF5-2A002B384297}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ACA6CFA-7E2C-4EA5-A8B0-7C328DA2F9FC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -549,7 +549,7 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>12.5</v>
+        <v>17.708333333333332</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -619,14 +619,14 @@
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="4" t="str">
         <f t="shared" ref="F7:F9" si="1">IF(D7&gt;=100,"Done!",IF(D7&gt;0,"In Progress","TODO"))</f>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.3">
@@ -634,15 +634,14 @@
         <v>9</v>
       </c>
       <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="str">
-        <f t="shared" ref="E8:E27" si="2">"-"</f>
-        <v>-</v>
+        <v>100</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F8" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>TODO</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.3">
@@ -653,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E8:E27" si="2">"-"</f>
         <v>-</v>
       </c>
       <c r="F9" s="4" t="str">

</xml_diff>

<commit_message>
[1E] Crop a imagem original implementada
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hsdyn-my.sharepoint.com/personal/bmonteiro_hsdyn_com/Documents/Documents/IMAVD_GRUPO_IMAGEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D8D2E38-A685-43CD-BA47-F43765DFE610}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11CB02FC-A73E-4010-B3D8-B6552F5863B7}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>47.916666666666664</v>
+        <v>52.083333333333336</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -693,15 +693,14 @@
         <v>13</v>
       </c>
       <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="str">
-        <f t="shared" ref="E10:E27" si="2">"-"</f>
-        <v>-</v>
+        <v>100</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
@@ -712,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E12:E27" si="2">"-"</f>
         <v>-</v>
       </c>
       <c r="F13" s="4" t="str">

</xml_diff>

<commit_message>
[1F] Desenvolvimento de salvar imagem cropada
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hsdyn-my.sharepoint.com/personal/bmonteiro_hsdyn_com/Documents/Documents/IMAVD_GRUPO_IMAGEM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11CB02FC-A73E-4010-B3D8-B6552F5863B7}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{4EFD24E4-FC80-4708-89D1-B6F3BA2D01A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F0B4B33-248B-4383-B93C-3517F2D99767}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -549,7 +549,7 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>52.083333333333336</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -708,15 +708,14 @@
         <v>14</v>
       </c>
       <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6" t="str">
-        <f t="shared" ref="E12:E27" si="2">"-"</f>
-        <v>-</v>
+        <v>100</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.3">
@@ -727,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="E13:E27" si="2">"-"</f>
         <v>-</v>
       </c>
       <c r="F14" s="4" t="str">

</xml_diff>

<commit_message>
[1M] Added Undo and Redo functionality (+ hotkeys and added buttons have disable/enable logic)
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TreeSource_Reps\Mestrado\1ano\2semestre\IMAVD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E18ACD6-6EAA-4A60-AFF5-B695512C652D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D5BC9F-45B3-40B2-B3FA-44BC2A2B5FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -248,7 +248,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -554,27 +638,27 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.3125" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>58.333333333333336</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+        <v>61.875</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,7 +672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -599,11 +683,11 @@
         <v>32</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f t="shared" ref="F5:F28" si="0">IF(D5&gt;=100,"Done!",IF(D5&gt;0,"In Progress","TODO"))</f>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+        <f>IF(D5&gt;=100,"Done!",IF(D5&gt;=90,"Almost there",IF(D5&gt;0,"In Progress","TODO")))</f>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -614,11 +698,11 @@
         <v>8</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f>IF(D6&gt;=100,"Done!",IF(D6&gt;0,"In Progress","TODO"))</f>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F6:F28" si="0">IF(D6&gt;=100,"Done!",IF(D6&gt;=90,"Almost there",IF(D6&gt;0,"In Progress","TODO")))</f>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -629,11 +713,11 @@
         <v>31</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f t="shared" ref="F7:F9" si="1">IF(D7&gt;=100,"Done!",IF(D7&gt;0,"In Progress","TODO"))</f>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -644,11 +728,11 @@
         <v>31</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -659,11 +743,11 @@
         <v>31</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
@@ -678,7 +762,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
@@ -693,7 +777,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -708,7 +792,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -723,7 +807,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -731,7 +815,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="6" t="str">
-        <f t="shared" ref="E14:E27" si="2">"-"</f>
+        <f t="shared" ref="E14:E27" si="1">"-"</f>
         <v>-</v>
       </c>
       <c r="F14" s="4" t="str">
@@ -739,7 +823,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -754,7 +838,7 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
@@ -769,7 +853,7 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
@@ -784,7 +868,7 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
@@ -792,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F18" s="4" t="str">
@@ -800,7 +884,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -808,7 +892,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F19" s="4" t="str">
@@ -816,23 +900,22 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
+        <v>90</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+        <v>Almost there</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
@@ -840,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F21" s="4" t="str">
@@ -848,7 +931,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -863,7 +946,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
@@ -878,7 +961,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
@@ -886,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F24" s="4" t="str">
@@ -894,7 +977,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
@@ -909,7 +992,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -917,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F26" s="4" t="str">
@@ -925,7 +1008,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
@@ -933,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
       <c r="F27" s="4" t="str">
@@ -941,33 +1024,46 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Done!</v>
+        <v>Almost there</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:F28">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"TODO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"Almost there"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F28">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Done!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implementação do brightness e do contraste
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E18ACD6-6EAA-4A60-AFF5-B695512C652D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836F533-9371-41B6-B08E-F53FD6F25DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,14 +151,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -243,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,7 +546,7 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +563,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>58.333333333333336</v>
+        <v>63.541666666666664</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -744,7 +736,7 @@
         <v>16</v>
       </c>
       <c r="D15" s="4">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>32</v>
@@ -759,14 +751,14 @@
         <v>17</v>
       </c>
       <c r="D16" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.3">
@@ -774,14 +766,14 @@
         <v>18</v>
       </c>
       <c r="D17" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implementação do contraste e brilho da imagem
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TreeSource_Reps\Mestrado\1ano\2semestre\IMAVD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D5BC9F-45B3-40B2-B3FA-44BC2A2B5FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633A4F8-A354-47E0-97DA-34AADEC9EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -248,7 +248,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -260,83 +260,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -638,27 +561,27 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.3125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5234375" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>61.875</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+        <v>67.083333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -672,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -687,7 +610,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -702,7 +625,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -717,7 +640,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -732,7 +655,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -747,7 +670,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
@@ -762,7 +685,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
@@ -777,7 +700,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -792,7 +715,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -807,7 +730,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -823,12 +746,12 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="4">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>32</v>
@@ -838,37 +761,37 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="7">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
@@ -884,7 +807,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -900,7 +823,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
@@ -915,7 +838,7 @@
         <v>Almost there</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
@@ -931,7 +854,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -946,7 +869,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
@@ -961,7 +884,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
@@ -977,7 +900,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
@@ -992,7 +915,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -1008,7 +931,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +947,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
@@ -1041,18 +964,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:F28">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"TODO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Almost there"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F28">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Done!"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implementação dos filtros red, green ou blue.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633A4F8-A354-47E0-97DA-34AADEC9EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C592DBD0-E656-4590-8365-DE2C8133917E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,7 +578,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>67.083333333333329</v>
+        <v>70.208333333333329</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -751,14 +751,14 @@
         <v>16</v>
       </c>
       <c r="D15" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[1G] Added zoom features, as well as vertical and horizontal panning (all with scroll events)
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TreeSource_Reps\Mestrado\1ano\2semestre\IMAVD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3503D77-503E-4918-ADED-E0EB51D1975F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4ED554-DCA9-47F1-9102-F8822189C015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -561,27 +561,27 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.3125" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>71.25</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+        <v>74.583333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -610,7 +610,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -625,7 +625,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -640,7 +640,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -655,7 +655,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -670,7 +670,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
@@ -685,7 +685,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
@@ -700,7 +700,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -715,7 +715,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -730,84 +730,83 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="4">
+        <v>80</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>In Progress</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4">
+        <v>100</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7">
+        <v>100</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4">
+        <v>100</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="4">
         <v>0</v>
       </c>
-      <c r="E14" s="6" t="str">
+      <c r="E18" s="6" t="str">
         <f t="shared" ref="E14:E27" si="1">"-"</f>
         <v>-</v>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>TODO</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="4">
-        <v>100</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="7">
-        <v>100</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4">
-        <v>100</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>Done!</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>TODO</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -823,7 +822,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
@@ -838,23 +837,22 @@
         <v>Almost there</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="4">
         <v>0</v>
       </c>
-      <c r="E21" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E21" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="F21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>TODO</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -869,7 +867,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
@@ -884,7 +882,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
@@ -900,7 +898,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
@@ -915,7 +913,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -930,7 +928,7 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
@@ -946,7 +944,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Conclusão da implementação do gamma
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hsdyn-my.sharepoint.com/personal/bmonteiro_hsdyn_com/Documents/Documents/IMAVD_GRUPO_IMAGEM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{6C4ED554-DCA9-47F1-9102-F8822189C015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D139B3F-7D9D-4E52-9703-5A9436ADB99D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9942AD9-A2E4-43D2-9629-EACA31348275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>74.583333333333329</v>
+        <v>77.708333333333329</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="6" t="str">
-        <f t="shared" ref="E18:E27" si="1">"-"</f>
+        <f t="shared" ref="E24:E27" si="1">"-"</f>
         <v>-</v>
       </c>
       <c r="F24" s="4" t="str">
@@ -916,14 +916,14 @@
         <v>26</v>
       </c>
       <c r="D26" s="4">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Inicialização da implementação do adicionar texto/imagem.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9942AD9-A2E4-43D2-9629-EACA31348275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7273615-795D-43E8-8213-7C0E1C3D61DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Alinea</t>
   </si>
@@ -561,7 +561,7 @@
   <dimension ref="C3:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +578,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>77.708333333333329</v>
+        <v>78.125</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -885,15 +885,14 @@
         <v>25</v>
       </c>
       <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="6" t="str">
-        <f t="shared" ref="E24:E27" si="1">"-"</f>
-        <v>-</v>
+        <v>10</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="F24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
+        <v>In Progress</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
@@ -934,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E24:E27" si="1">"-"</f>
         <v>-</v>
       </c>
       <c r="F27" s="4" t="str">

</xml_diff>

<commit_message>
Implementação do adicionar uma imagem à imagem atual
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7273615-795D-43E8-8213-7C0E1C3D61DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DAA8D1-E2FB-41EB-AB15-F26B6AF278C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,7 +578,7 @@
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>78.125</v>
+        <v>81.875</v>
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.3">
@@ -885,14 +885,14 @@
         <v>25</v>
       </c>
       <c r="D24" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>In Progress</v>
+        <v>Done!</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.3">
@@ -933,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="6" t="str">
-        <f t="shared" ref="E24:E27" si="1">"-"</f>
+        <f t="shared" ref="E27" si="1">"-"</f>
         <v>-</v>
       </c>
       <c r="F27" s="4" t="str">

</xml_diff>

<commit_message>
[1N] Redimension feature added. Some minor bugs to fix regarding the Absolute resizing.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mumbl\Documents\ISEP\Mestrado_SGM\IMAVD\IMAVD_GRUPO_IMAGEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TreeSource_Reps\Mestrado\1ano\2semestre\IMAVD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DAA8D1-E2FB-41EB-AB15-F26B6AF278C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7D6F8D-E332-46ED-86FE-9515DABBFCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Alinea</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>João</t>
+  </si>
+  <si>
+    <t>alguns bugs</t>
   </si>
 </sst>
 </file>
@@ -560,28 +563,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.3125" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5234375" customWidth="1"/>
+    <col min="7" max="7" width="12.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3">
         <f>SUM(D5:D28)/COUNT(D5:D28)</f>
-        <v>81.875</v>
-      </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+        <v>85.833333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
@@ -595,7 +599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -610,7 +614,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -625,7 +629,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
@@ -640,7 +644,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
@@ -655,7 +659,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
@@ -670,7 +674,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
@@ -685,7 +689,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
@@ -700,7 +704,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
@@ -715,7 +719,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
@@ -730,7 +734,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
@@ -745,7 +749,7 @@
         <v>In Progress</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
@@ -760,7 +764,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
@@ -775,7 +779,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" s="5" t="s">
         <v>18</v>
       </c>
@@ -790,7 +794,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
@@ -805,7 +809,7 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
@@ -820,37 +824,40 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="4">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Almost there</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+        <v>Done!</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>TODO</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+        <v>In Progress</v>
+      </c>
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="5" t="s">
         <v>23</v>
       </c>
@@ -865,7 +872,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="5" t="s">
         <v>24</v>
       </c>
@@ -880,7 +887,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
@@ -895,7 +902,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="5" t="s">
         <v>27</v>
       </c>
@@ -910,7 +917,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -925,7 +932,7 @@
         <v>Done!</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
@@ -941,19 +948,19 @@
         <v>TODO</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="4">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>Almost there</v>
+        <v>Done!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>